<commit_message>
importacao de tabela excel e metodo de criacao dos itens no banco
</commit_message>
<xml_diff>
--- a/backend/Pasta1.xlsx
+++ b/backend/Pasta1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Projetos_de_cursos\Projeto nex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Projetos_de_cursos\Projeto nex\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05EDA16A-83FA-47E9-9C1D-6D85DC2A1BA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EA5959-04D5-4DC8-921E-BEABD8319880}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{229624BB-88F0-46B5-A4A6-4C1D5E6EF485}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
   <si>
     <t>CPF</t>
   </si>
@@ -64,16 +64,192 @@
   </si>
   <si>
     <t>Em avaliação</t>
+  </si>
+  <si>
+    <t>282.279.300-01</t>
+  </si>
+  <si>
+    <t>282.279.300-02</t>
+  </si>
+  <si>
+    <t>282.279.300-03</t>
+  </si>
+  <si>
+    <t>282.279.300-04</t>
+  </si>
+  <si>
+    <t>282.279.300-05</t>
+  </si>
+  <si>
+    <t>282.279.300-06</t>
+  </si>
+  <si>
+    <t>282.279.300-07</t>
+  </si>
+  <si>
+    <t>282.279.300-08</t>
+  </si>
+  <si>
+    <t>282.279.300-09</t>
+  </si>
+  <si>
+    <t>282.279.300-10</t>
+  </si>
+  <si>
+    <t>282.279.300-11</t>
+  </si>
+  <si>
+    <t>282.279.300-12</t>
+  </si>
+  <si>
+    <t>282.279.300-13</t>
+  </si>
+  <si>
+    <t>282.279.300-14</t>
+  </si>
+  <si>
+    <t>282.279.300-15</t>
+  </si>
+  <si>
+    <t>282.279.300-16</t>
+  </si>
+  <si>
+    <t>282.279.300-17</t>
+  </si>
+  <si>
+    <t>282.279.300-18</t>
+  </si>
+  <si>
+    <t>282.279.300-19</t>
+  </si>
+  <si>
+    <t>282.279.300-20</t>
+  </si>
+  <si>
+    <t>282.279.300-21</t>
+  </si>
+  <si>
+    <t>282.279.300-22</t>
+  </si>
+  <si>
+    <t>282.279.300-23</t>
+  </si>
+  <si>
+    <t>282.279.300-24</t>
+  </si>
+  <si>
+    <t>282.279.300-25</t>
+  </si>
+  <si>
+    <t>282.279.300-26</t>
+  </si>
+  <si>
+    <t>282.279.300-27</t>
+  </si>
+  <si>
+    <t>282.279.300-28</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,8 +275,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B396572E-99A9-4959-88BC-D681D06E5AA6}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +651,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -493,7 +671,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -511,7 +689,529 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>44845</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>12000</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>44846</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>12001</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>44847</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>12002</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>44848</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>12003</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>44849</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>12004</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>44850</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>12005</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>44851</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>12006</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>44852</v>
+      </c>
+      <c r="D12">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>12007</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>44853</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>12008</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>44854</v>
+      </c>
+      <c r="D14">
+        <v>21</v>
+      </c>
+      <c r="E14">
+        <v>12009</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>44855</v>
+      </c>
+      <c r="D15">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <v>12010</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>44856</v>
+      </c>
+      <c r="D16">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>12011</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17">
+        <v>44857</v>
+      </c>
+      <c r="D17">
+        <v>24</v>
+      </c>
+      <c r="E17">
+        <v>12012</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>44858</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>12013</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19">
+        <v>44859</v>
+      </c>
+      <c r="D19">
+        <v>26</v>
+      </c>
+      <c r="E19">
+        <v>12014</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>44860</v>
+      </c>
+      <c r="D20">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>12015</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21">
+        <v>44861</v>
+      </c>
+      <c r="D21">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <v>12016</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22">
+        <v>44862</v>
+      </c>
+      <c r="D22">
+        <v>29</v>
+      </c>
+      <c r="E22">
+        <v>12017</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23">
+        <v>44863</v>
+      </c>
+      <c r="D23">
+        <v>30</v>
+      </c>
+      <c r="E23">
+        <v>12018</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24">
+        <v>44864</v>
+      </c>
+      <c r="D24">
+        <v>31</v>
+      </c>
+      <c r="E24">
+        <v>12019</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25">
+        <v>44865</v>
+      </c>
+      <c r="D25">
+        <v>32</v>
+      </c>
+      <c r="E25">
+        <v>12020</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>44866</v>
+      </c>
+      <c r="D26">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>12021</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27">
+        <v>44867</v>
+      </c>
+      <c r="D27">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>12022</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>44868</v>
+      </c>
+      <c r="D28">
+        <v>35</v>
+      </c>
+      <c r="E28">
+        <v>12023</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29">
+        <v>44869</v>
+      </c>
+      <c r="D29">
+        <v>36</v>
+      </c>
+      <c r="E29">
+        <v>12024</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30">
+        <v>44870</v>
+      </c>
+      <c r="D30">
+        <v>37</v>
+      </c>
+      <c r="E30">
+        <v>12025</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ajuste do banco de dados
</commit_message>
<xml_diff>
--- a/backend/Pasta1.xlsx
+++ b/backend/Pasta1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Projetos_de_cursos\Projeto nex\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EA5959-04D5-4DC8-921E-BEABD8319880}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F029E8A0-7C8A-429E-9C0D-BFD6FB213160}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{229624BB-88F0-46B5-A4A6-4C1D5E6EF485}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>CPF</t>
   </si>
@@ -275,10 +275,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B396572E-99A9-4959-88BC-D681D06E5AA6}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,10 +650,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>44844</v>
@@ -666,15 +665,15 @@
         <v>10000</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>44844</v>
@@ -686,527 +685,587 @@
         <v>10000</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>44845</v>
+        <v>44844</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>12000</v>
-      </c>
-      <c r="F5" s="2" t="s">
+        <v>10000</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>44846</v>
+        <v>44844</v>
       </c>
       <c r="D6">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>12001</v>
-      </c>
-      <c r="F6" s="2" t="s">
+        <v>10000</v>
+      </c>
+      <c r="F6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>44847</v>
+        <v>44844</v>
       </c>
       <c r="D7">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>12002</v>
-      </c>
-      <c r="F7" s="2" t="s">
+        <v>10000</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8">
-        <v>44848</v>
+        <v>44845</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>12003</v>
-      </c>
-      <c r="F8" s="2" t="s">
+        <v>12000</v>
+      </c>
+      <c r="F8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9">
-        <v>44849</v>
+        <v>44846</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E9">
-        <v>12004</v>
-      </c>
-      <c r="F9" s="2" t="s">
+        <v>12001</v>
+      </c>
+      <c r="F9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10">
-        <v>44850</v>
+        <v>44847</v>
       </c>
       <c r="D10">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E10">
-        <v>12005</v>
-      </c>
-      <c r="F10" s="2" t="s">
+        <v>12002</v>
+      </c>
+      <c r="F10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>44851</v>
+        <v>44848</v>
       </c>
       <c r="D11">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11">
-        <v>12006</v>
-      </c>
-      <c r="F11" s="2" t="s">
+        <v>12003</v>
+      </c>
+      <c r="F11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12">
-        <v>44852</v>
+        <v>44849</v>
       </c>
       <c r="D12">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E12">
-        <v>12007</v>
-      </c>
-      <c r="F12" s="2" t="s">
+        <v>12004</v>
+      </c>
+      <c r="F12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C13">
-        <v>44853</v>
+        <v>44850</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E13">
-        <v>12008</v>
-      </c>
-      <c r="F13" s="2" t="s">
+        <v>12005</v>
+      </c>
+      <c r="F13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14">
-        <v>44854</v>
+        <v>44851</v>
       </c>
       <c r="D14">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E14">
-        <v>12009</v>
-      </c>
-      <c r="F14" s="2" t="s">
+        <v>12006</v>
+      </c>
+      <c r="F14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C15">
-        <v>44855</v>
+        <v>44852</v>
       </c>
       <c r="D15">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E15">
-        <v>12010</v>
-      </c>
-      <c r="F15" s="2" t="s">
+        <v>12007</v>
+      </c>
+      <c r="F15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C16">
-        <v>44856</v>
+        <v>44853</v>
       </c>
       <c r="D16">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>12011</v>
-      </c>
-      <c r="F16" s="2" t="s">
+        <v>12008</v>
+      </c>
+      <c r="F16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17">
-        <v>44857</v>
+        <v>44854</v>
       </c>
       <c r="D17">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E17">
-        <v>12012</v>
-      </c>
-      <c r="F17" s="2" t="s">
+        <v>12009</v>
+      </c>
+      <c r="F17" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C18">
-        <v>44858</v>
+        <v>44855</v>
       </c>
       <c r="D18">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E18">
-        <v>12013</v>
-      </c>
-      <c r="F18" s="2" t="s">
+        <v>12010</v>
+      </c>
+      <c r="F18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19">
-        <v>44859</v>
+        <v>44856</v>
       </c>
       <c r="D19">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E19">
-        <v>12014</v>
-      </c>
-      <c r="F19" s="2" t="s">
+        <v>12011</v>
+      </c>
+      <c r="F19" t="s">
         <v>12</v>
       </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20">
-        <v>44860</v>
+        <v>44857</v>
       </c>
       <c r="D20">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E20">
-        <v>12015</v>
-      </c>
-      <c r="F20" s="2" t="s">
+        <v>12012</v>
+      </c>
+      <c r="F20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C21">
-        <v>44861</v>
+        <v>44858</v>
       </c>
       <c r="D21">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E21">
-        <v>12016</v>
-      </c>
-      <c r="F21" s="2" t="s">
+        <v>12013</v>
+      </c>
+      <c r="F21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22">
-        <v>44862</v>
+        <v>44859</v>
       </c>
       <c r="D22">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E22">
-        <v>12017</v>
-      </c>
-      <c r="F22" s="2" t="s">
+        <v>12014</v>
+      </c>
+      <c r="F22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C23">
-        <v>44863</v>
+        <v>44860</v>
       </c>
       <c r="D23">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E23">
-        <v>12018</v>
-      </c>
-      <c r="F23" s="2" t="s">
+        <v>12015</v>
+      </c>
+      <c r="F23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C24">
-        <v>44864</v>
+        <v>44861</v>
       </c>
       <c r="D24">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E24">
-        <v>12019</v>
-      </c>
-      <c r="F24" s="2" t="s">
+        <v>12016</v>
+      </c>
+      <c r="F24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C25">
-        <v>44865</v>
+        <v>44862</v>
       </c>
       <c r="D25">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25">
-        <v>12020</v>
-      </c>
-      <c r="F25" s="2" t="s">
+        <v>12017</v>
+      </c>
+      <c r="F25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C26">
-        <v>44866</v>
+        <v>44863</v>
       </c>
       <c r="D26">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E26">
-        <v>12021</v>
-      </c>
-      <c r="F26" s="2" t="s">
+        <v>12018</v>
+      </c>
+      <c r="F26" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C27">
-        <v>44867</v>
+        <v>44864</v>
       </c>
       <c r="D27">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E27">
-        <v>12022</v>
-      </c>
-      <c r="F27" s="2" t="s">
+        <v>12019</v>
+      </c>
+      <c r="F27" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28">
-        <v>44868</v>
+        <v>44865</v>
       </c>
       <c r="D28">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E28">
-        <v>12023</v>
-      </c>
-      <c r="F28" s="2" t="s">
+        <v>12020</v>
+      </c>
+      <c r="F28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C29">
-        <v>44869</v>
+        <v>44866</v>
       </c>
       <c r="D29">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E29">
-        <v>12024</v>
-      </c>
-      <c r="F29" s="2" t="s">
+        <v>12021</v>
+      </c>
+      <c r="F29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30">
+        <v>44867</v>
+      </c>
+      <c r="D30">
+        <v>34</v>
+      </c>
+      <c r="E30">
+        <v>12022</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31">
+        <v>44868</v>
+      </c>
+      <c r="D31">
+        <v>35</v>
+      </c>
+      <c r="E31">
+        <v>12023</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32">
+        <v>44869</v>
+      </c>
+      <c r="D32">
+        <v>36</v>
+      </c>
+      <c r="E32">
+        <v>12024</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>40</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>65</v>
       </c>
-      <c r="C30">
+      <c r="C33">
         <v>44870</v>
       </c>
-      <c r="D30">
+      <c r="D33">
         <v>37</v>
       </c>
-      <c r="E30">
+      <c r="E33">
         <v>12025</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F33" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>